<commit_message>
arreglar detalles de promociones
</commit_message>
<xml_diff>
--- a/core/reportes/bases/resumen.xlsx
+++ b/core/reportes/bases/resumen.xlsx
@@ -539,6 +539,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,9 +564,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -946,10 +946,10 @@
   <dimension ref="A3:AC109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:P5"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8:D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,59 +974,59 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
     </row>
     <row r="6" spans="1:29" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="35" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="36"/>
-      <c r="L6" s="32" t="s">
+      <c r="K6" s="37"/>
+      <c r="L6" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="33"/>
-      <c r="N6" s="32" t="s">
+      <c r="M6" s="34"/>
+      <c r="N6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="33"/>
+      <c r="O6" s="34"/>
       <c r="P6" s="31" t="s">
         <v>6</v>
       </c>
@@ -1087,9 +1087,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="8"/>
@@ -1113,9 +1111,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D9" s="6"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="8"/>
@@ -1144,9 +1140,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="8"/>
@@ -1175,9 +1169,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D11" s="6"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="8"/>
@@ -1206,9 +1198,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D12" s="6"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="8"/>
@@ -1237,9 +1227,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D13" s="6"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="8"/>
@@ -1268,9 +1256,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D14" s="6"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="8"/>
@@ -1291,9 +1277,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D15" s="6"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="8"/>
@@ -1320,9 +1304,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D16" s="6"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="8"/>
@@ -1346,9 +1328,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D17" s="6"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="8"/>
@@ -1377,9 +1357,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D18" s="6"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="8"/>
@@ -1408,9 +1386,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D19" s="6"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="8"/>
@@ -1439,9 +1415,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D20" s="6"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="8"/>
@@ -1470,9 +1444,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D21" s="6"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="8"/>
@@ -1501,9 +1473,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D22" s="6"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="8"/>
@@ -1524,9 +1494,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D23" s="6"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="8"/>
@@ -1550,9 +1518,7 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D24" s="6"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="8"/>
@@ -1577,9 +1543,7 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D25" s="6"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="8"/>
@@ -1604,9 +1568,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D26" s="6"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="8"/>
@@ -1631,9 +1593,7 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D27" s="6"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="8"/>
@@ -1658,9 +1618,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D28" s="6"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="8"/>
@@ -1685,9 +1643,7 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D29" s="6"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="8"/>
@@ -1708,9 +1664,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D30" s="6"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="8"/>
@@ -1731,9 +1685,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D31" s="6"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="8"/>
@@ -1754,9 +1706,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D32" s="6"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="8"/>
@@ -1780,9 +1730,7 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D33" s="6"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="8"/>
@@ -1806,9 +1754,7 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D34" s="6"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="8"/>
@@ -1837,9 +1783,7 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D35" s="6"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
       <c r="G35" s="8"/>
@@ -1868,9 +1812,7 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D36" s="6"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="8"/>
@@ -1899,9 +1841,7 @@
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D37" s="6"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="8"/>
@@ -1930,9 +1870,7 @@
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D38" s="6"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="8"/>
@@ -1961,9 +1899,7 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D39" s="6"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
       <c r="G39" s="8"/>
@@ -1984,9 +1920,7 @@
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D40" s="6"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
       <c r="G40" s="8"/>
@@ -2007,9 +1941,7 @@
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D41" s="6"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="8"/>
@@ -2030,9 +1962,7 @@
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D42" s="6"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="8"/>
@@ -2053,9 +1983,7 @@
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="7"/>
-      <c r="D43" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D43" s="6"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
       <c r="G43" s="8"/>
@@ -2076,9 +2004,7 @@
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D44" s="6"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
       <c r="G44" s="8"/>
@@ -2099,9 +2025,7 @@
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="7"/>
-      <c r="D45" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D45" s="6"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
       <c r="G45" s="8"/>
@@ -2122,9 +2046,7 @@
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="7"/>
-      <c r="D46" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D46" s="6"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
       <c r="G46" s="8"/>
@@ -2145,9 +2067,7 @@
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="7"/>
-      <c r="D47" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D47" s="6"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
       <c r="G47" s="8"/>
@@ -2168,9 +2088,7 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="7"/>
-      <c r="D48" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D48" s="6"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
       <c r="G48" s="8"/>
@@ -2191,9 +2109,7 @@
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="7"/>
-      <c r="D49" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D49" s="6"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
       <c r="G49" s="8"/>
@@ -2214,9 +2130,7 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="7"/>
-      <c r="D50" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D50" s="6"/>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
       <c r="G50" s="8"/>
@@ -2237,9 +2151,7 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="7"/>
-      <c r="D51" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D51" s="6"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="8"/>
@@ -2260,9 +2172,7 @@
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="7"/>
-      <c r="D52" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D52" s="6"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
       <c r="G52" s="8"/>
@@ -2283,9 +2193,7 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="7"/>
-      <c r="D53" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D53" s="6"/>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
       <c r="G53" s="8"/>
@@ -2306,9 +2214,7 @@
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="7"/>
-      <c r="D54" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D54" s="6"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
       <c r="G54" s="8"/>
@@ -2329,9 +2235,7 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="7"/>
-      <c r="D55" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D55" s="6"/>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
       <c r="G55" s="8"/>
@@ -2352,9 +2256,7 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="7"/>
-      <c r="D56" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D56" s="6"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
       <c r="G56" s="8"/>
@@ -2375,9 +2277,7 @@
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="7"/>
-      <c r="D57" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D57" s="6"/>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
       <c r="G57" s="8"/>
@@ -2398,9 +2298,7 @@
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="7"/>
-      <c r="D58" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D58" s="6"/>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
       <c r="G58" s="8"/>
@@ -2421,9 +2319,7 @@
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="7"/>
-      <c r="D59" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D59" s="6"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="8"/>
@@ -2444,9 +2340,7 @@
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="7"/>
-      <c r="D60" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D60" s="6"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
       <c r="G60" s="8"/>
@@ -2467,9 +2361,7 @@
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="7"/>
-      <c r="D61" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D61" s="6"/>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
       <c r="G61" s="8"/>
@@ -2490,9 +2382,7 @@
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="7"/>
-      <c r="D62" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D62" s="6"/>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
       <c r="G62" s="8"/>
@@ -2513,9 +2403,7 @@
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="7"/>
-      <c r="D63" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D63" s="6"/>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
       <c r="G63" s="8"/>
@@ -2536,9 +2424,7 @@
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="7"/>
-      <c r="D64" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D64" s="6"/>
       <c r="E64" s="9"/>
       <c r="F64" s="9"/>
       <c r="G64" s="8"/>
@@ -2559,9 +2445,7 @@
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="7"/>
-      <c r="D65" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D65" s="6"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
       <c r="G65" s="8"/>
@@ -2582,9 +2466,7 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="7"/>
-      <c r="D66" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D66" s="6"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
       <c r="G66" s="8"/>
@@ -2605,9 +2487,7 @@
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="7"/>
-      <c r="D67" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D67" s="6"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="8"/>
@@ -2628,9 +2508,7 @@
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="7"/>
-      <c r="D68" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D68" s="6"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
       <c r="G68" s="8"/>
@@ -2651,9 +2529,7 @@
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="7"/>
-      <c r="D69" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D69" s="6"/>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="8"/>
@@ -2674,9 +2550,7 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D70" s="6"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="8"/>
@@ -2697,9 +2571,7 @@
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="7"/>
-      <c r="D71" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D71" s="6"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="8"/>
@@ -2720,9 +2592,7 @@
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="7"/>
-      <c r="D72" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D72" s="6"/>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="8"/>
@@ -2743,9 +2613,7 @@
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="7"/>
-      <c r="D73" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D73" s="6"/>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
       <c r="G73" s="8"/>
@@ -2766,9 +2634,7 @@
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="7"/>
-      <c r="D74" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D74" s="6"/>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
       <c r="G74" s="8"/>
@@ -2789,9 +2655,7 @@
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="7"/>
-      <c r="D75" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D75" s="6"/>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
       <c r="G75" s="8"/>
@@ -2812,9 +2676,7 @@
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="7"/>
-      <c r="D76" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D76" s="6"/>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
       <c r="G76" s="8"/>
@@ -2835,9 +2697,7 @@
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="7"/>
-      <c r="D77" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D77" s="6"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
       <c r="G77" s="8"/>
@@ -2858,9 +2718,7 @@
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="7"/>
-      <c r="D78" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D78" s="6"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
       <c r="G78" s="8"/>
@@ -2881,9 +2739,7 @@
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="7"/>
-      <c r="D79" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D79" s="6"/>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
       <c r="G79" s="8"/>
@@ -2904,9 +2760,7 @@
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="7"/>
-      <c r="D80" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D80" s="6"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
       <c r="G80" s="8"/>
@@ -2927,9 +2781,7 @@
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="7"/>
-      <c r="D81" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D81" s="6"/>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
       <c r="G81" s="8"/>
@@ -2950,9 +2802,7 @@
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="7"/>
-      <c r="D82" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D82" s="6"/>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
       <c r="G82" s="8"/>
@@ -2973,9 +2823,7 @@
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="7"/>
-      <c r="D83" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D83" s="6"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
       <c r="G83" s="8"/>
@@ -2996,9 +2844,7 @@
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="7"/>
-      <c r="D84" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D84" s="6"/>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
       <c r="G84" s="8"/>
@@ -3019,9 +2865,7 @@
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="7"/>
-      <c r="D85" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D85" s="6"/>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
       <c r="G85" s="8"/>
@@ -3042,9 +2886,7 @@
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="7"/>
-      <c r="D86" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D86" s="6"/>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
       <c r="G86" s="8"/>
@@ -3065,9 +2907,7 @@
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="7"/>
-      <c r="D87" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D87" s="6"/>
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
       <c r="G87" s="8"/>
@@ -3088,9 +2928,7 @@
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="7"/>
-      <c r="D88" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D88" s="6"/>
       <c r="E88" s="9"/>
       <c r="F88" s="9"/>
       <c r="G88" s="8"/>
@@ -3111,9 +2949,7 @@
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="7"/>
-      <c r="D89" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D89" s="6"/>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
       <c r="G89" s="8"/>
@@ -3134,9 +2970,7 @@
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="7"/>
-      <c r="D90" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D90" s="6"/>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
       <c r="G90" s="8"/>
@@ -3157,9 +2991,7 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="D91" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D91" s="6"/>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
       <c r="G91" s="2"/>
@@ -3180,9 +3012,7 @@
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
-      <c r="D92" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D92" s="6"/>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
       <c r="G92" s="2"/>
@@ -3203,9 +3033,7 @@
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
-      <c r="D93" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D93" s="6"/>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
       <c r="G93" s="2"/>
@@ -3226,9 +3054,7 @@
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
-      <c r="D94" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D94" s="6"/>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
       <c r="G94" s="2"/>
@@ -3249,9 +3075,7 @@
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="D95" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D95" s="6"/>
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
       <c r="G95" s="2"/>
@@ -3272,9 +3096,7 @@
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
-      <c r="D96" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D96" s="6"/>
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
       <c r="G96" s="2"/>
@@ -3295,9 +3117,7 @@
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
-      <c r="D97" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D97" s="6"/>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
       <c r="G97" s="2"/>
@@ -3318,9 +3138,7 @@
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
-      <c r="D98" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D98" s="6"/>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
       <c r="G98" s="2"/>
@@ -3341,9 +3159,7 @@
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
-      <c r="D99" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D99" s="6"/>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
       <c r="G99" s="2"/>
@@ -3364,9 +3180,7 @@
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D100" s="6"/>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
       <c r="G100" s="2"/>
@@ -3387,9 +3201,7 @@
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
-      <c r="D101" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D101" s="6"/>
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
       <c r="G101" s="2"/>
@@ -3410,9 +3222,7 @@
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
-      <c r="D102" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D102" s="6"/>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
       <c r="G102" s="2"/>
@@ -3433,9 +3243,7 @@
       </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
-      <c r="D103" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D103" s="6"/>
       <c r="E103" s="9"/>
       <c r="F103" s="9"/>
       <c r="G103" s="2"/>
@@ -3456,9 +3264,7 @@
       </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
-      <c r="D104" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D104" s="6"/>
       <c r="E104" s="9"/>
       <c r="F104" s="9"/>
       <c r="G104" s="2"/>
@@ -3479,9 +3285,7 @@
       </c>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
-      <c r="D105" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D105" s="6"/>
       <c r="E105" s="9"/>
       <c r="F105" s="9"/>
       <c r="G105" s="2"/>
@@ -3502,9 +3306,7 @@
       </c>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
-      <c r="D106" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D106" s="6"/>
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
       <c r="G106" s="2"/>
@@ -3525,9 +3327,7 @@
       </c>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
-      <c r="D107" s="6">
-        <v>36526</v>
-      </c>
+      <c r="D107" s="6"/>
       <c r="E107" s="9"/>
       <c r="F107" s="9"/>
       <c r="G107" s="2"/>
@@ -3582,9 +3382,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3702,25 +3505,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9B18B5C-CBA8-4FC0-9D85-84EF271EEF94}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA3F4D73-C9E3-4457-9228-79FCDA4E5586}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3742,9 +3535,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA3F4D73-C9E3-4457-9228-79FCDA4E5586}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9B18B5C-CBA8-4FC0-9D85-84EF271EEF94}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>